<commit_message>
convert µmoles to nmoles
</commit_message>
<xml_diff>
--- a/data/20251017/pnitroaniline_stdcurve.xlsx
+++ b/data/20251017/pnitroaniline_stdcurve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinsse/Documents/GitHub/platereader-plotting/data/20251017/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CD7F466-89F2-0247-8283-C468F3155BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77B16AE-E720-D04D-8432-F1223DEF980D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="10280" windowHeight="17480" xr2:uid="{97FCA1A2-ED69-1946-A5F2-02ADA5B08B2B}"/>
   </bookViews>
@@ -63,7 +63,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +97,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE8F3FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DBCE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9E0F4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -128,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -143,6 +155,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -479,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCA38CE-DEC1-8445-AC9A-2279C7B18442}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B23" sqref="B23:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,6 +569,174 @@
         <v>0.15</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>500</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>250</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1.6870000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>125</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>62.5</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.54800000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>31.25</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.41099999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>15.63</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>500</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3.2170000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>250</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1.6870000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>125</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>62.5</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>31.25</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.40200000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>15.63</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.30599999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>500</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3.1629999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>250</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1.6639999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>125</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>62.5</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.54500000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>31.25</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>15.63</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0.14499999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>